<commit_message>
Xu ly ca Bao Ve
</commit_message>
<xml_diff>
--- a/convert/Cong_thang_9.xlsx
+++ b/convert/Cong_thang_9.xlsx
@@ -6312,7 +6312,7 @@
         <v>55</v>
       </c>
       <c r="AB12">
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="AC12" t="s">
         <v>46</v>
@@ -7049,7 +7049,7 @@
         <v>46</v>
       </c>
       <c r="Z16">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB16">
         <v>12</v>
@@ -8007,7 +8007,7 @@
         <v>46</v>
       </c>
       <c r="AL21">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AM21" t="s">
         <v>46</v>
@@ -8848,7 +8848,7 @@
         <v>46</v>
       </c>
       <c r="H26">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="I26" t="s">
         <v>36</v>
@@ -8887,13 +8887,13 @@
         <v>46</v>
       </c>
       <c r="V26">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="W26" t="s">
         <v>46</v>
       </c>
       <c r="X26">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Y26" t="s">
         <v>46</v>
@@ -8920,7 +8920,7 @@
         <v>46</v>
       </c>
       <c r="AH26">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AI26" t="s">
         <v>46</v>
@@ -8938,7 +8938,7 @@
         <v>46</v>
       </c>
       <c r="AN26">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AP26">
         <v>10</v>
@@ -8965,7 +8965,7 @@
         <v>46</v>
       </c>
       <c r="AX26">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AY26" t="s">
         <v>46</v>
@@ -8992,7 +8992,7 @@
         <v>46</v>
       </c>
       <c r="BH26">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BI26" t="s">
         <v>46</v>
@@ -9997,7 +9997,7 @@
         <v>50</v>
       </c>
       <c r="V32">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="W32" t="s">
         <v>50</v>
@@ -10018,7 +10018,7 @@
         <v>50</v>
       </c>
       <c r="AD32">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AE32" t="s">
         <v>50</v>
@@ -10042,7 +10042,7 @@
         <v>50</v>
       </c>
       <c r="AL32">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AM32" t="s">
         <v>50</v>
@@ -10063,7 +10063,7 @@
         <v>50</v>
       </c>
       <c r="AT32">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AU32" t="s">
         <v>50</v>
@@ -10096,13 +10096,13 @@
         <v>50</v>
       </c>
       <c r="BF32">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BG32" t="s">
         <v>50</v>
       </c>
       <c r="BH32">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BI32" t="s">
         <v>50</v>
@@ -12316,7 +12316,7 @@
         <v>46</v>
       </c>
       <c r="BF44">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="BG44" t="s">
         <v>46</v>
@@ -12441,7 +12441,7 @@
         <v>46</v>
       </c>
       <c r="AJ45">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AK45" t="s">
         <v>46</v>
@@ -13232,7 +13232,7 @@
         <v>46</v>
       </c>
       <c r="BB49">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="BD49">
         <v>12</v>
@@ -13679,7 +13679,7 @@
         <v>50</v>
       </c>
       <c r="P52">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="Q52" t="s">
         <v>50</v>
@@ -13697,7 +13697,7 @@
         <v>50</v>
       </c>
       <c r="V52">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="W52" t="s">
         <v>50</v>
@@ -13730,25 +13730,25 @@
         <v>50</v>
       </c>
       <c r="AH52">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AI52" t="s">
         <v>50</v>
       </c>
       <c r="AJ52">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AK52" t="s">
         <v>50</v>
       </c>
       <c r="AL52">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AM52" t="s">
         <v>50</v>
       </c>
       <c r="AN52">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AP52">
         <v>0</v>
@@ -13781,7 +13781,7 @@
         <v>50</v>
       </c>
       <c r="AZ52">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BA52" t="s">
         <v>35</v>
@@ -13796,7 +13796,7 @@
         <v>50</v>
       </c>
       <c r="BF52">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BG52" t="s">
         <v>50</v>
@@ -13808,7 +13808,7 @@
         <v>50</v>
       </c>
       <c r="BJ52">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BK52" t="s">
         <v>50</v>
@@ -14419,7 +14419,7 @@
         <v>46</v>
       </c>
       <c r="P56">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="Q56" t="s">
         <v>46</v>
@@ -14464,7 +14464,7 @@
         <v>46</v>
       </c>
       <c r="AF56">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AG56" t="s">
         <v>46</v>
@@ -16505,7 +16505,7 @@
         <v>50</v>
       </c>
       <c r="AH67">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AI67" t="s">
         <v>50</v>
@@ -16526,7 +16526,7 @@
         <v>0</v>
       </c>
       <c r="AP67">
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="AQ67" t="s">
         <v>50</v>
@@ -18367,7 +18367,7 @@
         <v>46</v>
       </c>
       <c r="AL77">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AM77" t="s">
         <v>46</v>
@@ -18937,7 +18937,7 @@
         <v>46</v>
       </c>
       <c r="AR80">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AS80" t="s">
         <v>46</v>
@@ -18967,7 +18967,7 @@
         <v>46</v>
       </c>
       <c r="BB80">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="BD80">
         <v>12</v>
@@ -18994,7 +18994,7 @@
         <v>45</v>
       </c>
       <c r="BL80">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BM80" t="s">
         <v>45</v>
@@ -19364,13 +19364,13 @@
         <v>50</v>
       </c>
       <c r="BL82">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BM82" t="s">
         <v>50</v>
       </c>
       <c r="BN82">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="83" spans="1:66">
@@ -19492,7 +19492,7 @@
         <v>46</v>
       </c>
       <c r="AR83">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="AS83" t="s">
         <v>46</v>
@@ -19531,7 +19531,7 @@
         <v>46</v>
       </c>
       <c r="BF83">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BG83" t="s">
         <v>46</v>
@@ -19629,7 +19629,7 @@
         <v>46</v>
       </c>
       <c r="Z84">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AB84">
         <v>0</v>
@@ -19784,7 +19784,7 @@
         <v>50</v>
       </c>
       <c r="P85">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="Q85" t="s">
         <v>50</v>
@@ -19802,7 +19802,7 @@
         <v>50</v>
       </c>
       <c r="V85">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="W85" t="s">
         <v>50</v>
@@ -19823,13 +19823,13 @@
         <v>50</v>
       </c>
       <c r="AD85">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AE85" t="s">
         <v>50</v>
       </c>
       <c r="AF85">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AG85" t="s">
         <v>50</v>
@@ -19841,7 +19841,7 @@
         <v>50</v>
       </c>
       <c r="AJ85">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AK85" t="s">
         <v>50</v>
@@ -19862,7 +19862,7 @@
         <v>50</v>
       </c>
       <c r="AR85">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AS85" t="s">
         <v>50</v>
@@ -19886,7 +19886,7 @@
         <v>50</v>
       </c>
       <c r="AZ85">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BA85" t="s">
         <v>50</v>
@@ -19901,13 +19901,13 @@
         <v>50</v>
       </c>
       <c r="BF85">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BG85" t="s">
         <v>50</v>
       </c>
       <c r="BH85">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BI85" t="s">
         <v>50</v>
@@ -19919,7 +19919,7 @@
         <v>50</v>
       </c>
       <c r="BL85">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BM85" t="s">
         <v>50</v>
@@ -20518,31 +20518,31 @@
         <v>0</v>
       </c>
       <c r="N89">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="O89" t="s">
         <v>46</v>
       </c>
       <c r="P89">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="Q89" t="s">
         <v>46</v>
       </c>
       <c r="R89">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S89" t="s">
         <v>46</v>
       </c>
       <c r="T89">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="U89" t="s">
         <v>46</v>
       </c>
       <c r="V89">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="W89" t="s">
         <v>46</v>
@@ -20563,7 +20563,7 @@
         <v>46</v>
       </c>
       <c r="AD89">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AE89" t="s">
         <v>45</v>
@@ -20575,7 +20575,7 @@
         <v>45</v>
       </c>
       <c r="AH89">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AI89" t="s">
         <v>45</v>
@@ -20596,13 +20596,13 @@
         <v>3</v>
       </c>
       <c r="AP89">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AQ89" t="s">
         <v>46</v>
       </c>
       <c r="AR89">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AS89" t="s">
         <v>46</v>
@@ -20641,7 +20641,7 @@
         <v>45</v>
       </c>
       <c r="BF89">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BG89" t="s">
         <v>45</v>
@@ -21294,7 +21294,7 @@
         <v>46</v>
       </c>
       <c r="Z93">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AB93">
         <v>0</v>
@@ -21488,7 +21488,7 @@
         <v>50</v>
       </c>
       <c r="AD94">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AE94" t="s">
         <v>50</v>
@@ -21506,7 +21506,7 @@
         <v>50</v>
       </c>
       <c r="AJ94">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AK94" t="s">
         <v>50</v>
@@ -21572,7 +21572,7 @@
         <v>50</v>
       </c>
       <c r="BH94">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BI94" t="s">
         <v>50</v>
@@ -22276,7 +22276,7 @@
         <v>46</v>
       </c>
       <c r="AT98">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AU98" t="s">
         <v>46</v>
@@ -22309,7 +22309,7 @@
         <v>46</v>
       </c>
       <c r="BF98">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="BG98" t="s">
         <v>46</v>
@@ -22941,7 +22941,7 @@
         <v>46</v>
       </c>
       <c r="R102">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="S102" t="s">
         <v>46</v>
@@ -23720,7 +23720,7 @@
         <v>46</v>
       </c>
       <c r="AF106">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AG106" t="s">
         <v>46</v>
@@ -25251,7 +25251,7 @@
         <v>46</v>
       </c>
       <c r="AX114">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AY114" t="s">
         <v>35</v>
@@ -26916,7 +26916,7 @@
         <v>46</v>
       </c>
       <c r="AX123">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AY123" t="s">
         <v>46</v>
@@ -26943,7 +26943,7 @@
         <v>46</v>
       </c>
       <c r="BH123">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BI123" t="s">
         <v>46</v>
@@ -27038,7 +27038,7 @@
         <v>0</v>
       </c>
       <c r="AB124">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="AC124" t="s">
         <v>46</v>
@@ -27116,7 +27116,7 @@
         <v>0</v>
       </c>
       <c r="BD124">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="BE124" t="s">
         <v>50</v>
@@ -27235,7 +27235,7 @@
         <v>46</v>
       </c>
       <c r="AF125">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="AG125" t="s">
         <v>46</v>
@@ -27757,7 +27757,7 @@
         <v>46</v>
       </c>
       <c r="T128">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="U128" t="s">
         <v>35</v>
@@ -27769,7 +27769,7 @@
         <v>46</v>
       </c>
       <c r="X128">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="Y128" t="s">
         <v>35</v>
@@ -28372,7 +28372,7 @@
         <v>4</v>
       </c>
       <c r="AP131">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="AQ131" t="s">
         <v>45</v>
@@ -28575,7 +28575,7 @@
         <v>46</v>
       </c>
       <c r="AV132">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AW132" t="s">
         <v>35</v>
@@ -29040,7 +29040,7 @@
         <v>46</v>
       </c>
       <c r="P135">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="Q135" t="s">
         <v>46</v>
@@ -29118,7 +29118,7 @@
         <v>46</v>
       </c>
       <c r="AR135">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="AS135" t="s">
         <v>46</v>
@@ -30088,7 +30088,7 @@
         <v>46</v>
       </c>
       <c r="BH140">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BI140" t="s">
         <v>46</v>
@@ -30896,7 +30896,7 @@
         <v>46</v>
       </c>
       <c r="R145">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="S145" t="s">
         <v>46</v>
@@ -30980,7 +30980,7 @@
         <v>46</v>
       </c>
       <c r="AV145">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AW145" t="s">
         <v>35</v>
@@ -30998,7 +30998,7 @@
         <v>46</v>
       </c>
       <c r="BB145">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BD145">
         <v>12</v>
@@ -31299,7 +31299,7 @@
         <v>46</v>
       </c>
       <c r="AD147">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AE147" t="s">
         <v>46</v>
@@ -32618,7 +32618,7 @@
         <v>46</v>
       </c>
       <c r="AL154">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AM154" t="s">
         <v>46</v>
@@ -33021,7 +33021,7 @@
         <v>46</v>
       </c>
       <c r="AX156">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AY156" t="s">
         <v>46</v>
@@ -34799,7 +34799,7 @@
         <v>46</v>
       </c>
       <c r="X166">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="Y166" t="s">
         <v>46</v>
@@ -37741,7 +37741,7 @@
         <v>46</v>
       </c>
       <c r="R182">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="S182" t="s">
         <v>46</v>
@@ -37843,7 +37843,7 @@
         <v>46</v>
       </c>
       <c r="BB182">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BD182">
         <v>0</v>
@@ -37858,7 +37858,7 @@
         <v>46</v>
       </c>
       <c r="BH182">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="BI182" t="s">
         <v>46</v>
@@ -37870,7 +37870,7 @@
         <v>46</v>
       </c>
       <c r="BL182">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BM182" t="s">
         <v>46</v>
@@ -39412,7 +39412,7 @@
         <v>46</v>
       </c>
       <c r="T191">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="U191" t="s">
         <v>46</v>
@@ -40090,7 +40090,7 @@
         <v>46</v>
       </c>
       <c r="BL194">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BM194" t="s">
         <v>46</v>
@@ -41835,7 +41835,7 @@
         <v>45</v>
       </c>
       <c r="Z204">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AB204">
         <v>0</v>
@@ -41934,7 +41934,7 @@
         <v>46</v>
       </c>
       <c r="BJ204">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BK204" t="s">
         <v>46</v>
@@ -42035,7 +42035,7 @@
         <v>46</v>
       </c>
       <c r="AF205">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AG205" t="s">
         <v>46</v>
@@ -42563,7 +42563,7 @@
         <v>46</v>
       </c>
       <c r="V208">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="W208" t="s">
         <v>46</v>
@@ -42608,7 +42608,7 @@
         <v>46</v>
       </c>
       <c r="AL208">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AM208" t="s">
         <v>46</v>
@@ -42629,7 +42629,7 @@
         <v>46</v>
       </c>
       <c r="AT208">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="AU208" t="s">
         <v>46</v>
@@ -42656,7 +42656,7 @@
         <v>4</v>
       </c>
       <c r="BD208">
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="BE208" t="s">
         <v>46</v>
@@ -43918,13 +43918,13 @@
         <v>50</v>
       </c>
       <c r="AR215">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="AS215" t="s">
         <v>50</v>
       </c>
       <c r="AT215">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AU215" t="s">
         <v>50</v>
@@ -45323,7 +45323,7 @@
         <v>0</v>
       </c>
       <c r="N223">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="O223" t="s">
         <v>46</v>
@@ -45392,13 +45392,13 @@
         <v>45</v>
       </c>
       <c r="AL223">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AM223" t="s">
         <v>45</v>
       </c>
       <c r="AN223">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AP223">
         <v>3</v>
@@ -45407,7 +45407,7 @@
         <v>46</v>
       </c>
       <c r="AR223">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AS223" t="s">
         <v>46</v>
@@ -46093,13 +46093,13 @@
         <v>45</v>
       </c>
       <c r="X227">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="Y227" t="s">
         <v>45</v>
       </c>
       <c r="Z227">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AB227">
         <v>3</v>
@@ -46108,13 +46108,13 @@
         <v>46</v>
       </c>
       <c r="AD227">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AE227" t="s">
         <v>46</v>
       </c>
       <c r="AF227">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AG227" t="s">
         <v>46</v>
@@ -46132,13 +46132,13 @@
         <v>46</v>
       </c>
       <c r="AL227">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AM227" t="s">
         <v>46</v>
       </c>
       <c r="AN227">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AP227">
         <v>0</v>
@@ -46177,7 +46177,7 @@
         <v>45</v>
       </c>
       <c r="BB227">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BD227">
         <v>3</v>
@@ -46210,7 +46210,7 @@
         <v>46</v>
       </c>
       <c r="BN227">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="228" spans="1:66">
@@ -46356,7 +46356,7 @@
         <v>46</v>
       </c>
       <c r="AZ228">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BA228" t="s">
         <v>46</v>
@@ -49098,7 +49098,7 @@
         <v>46</v>
       </c>
       <c r="AN243">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="AP243">
         <v>8</v>
@@ -49131,7 +49131,7 @@
         <v>46</v>
       </c>
       <c r="AZ243">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BA243" t="s">
         <v>46</v>
@@ -49444,13 +49444,13 @@
         <v>50</v>
       </c>
       <c r="AF245">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AG245" t="s">
         <v>50</v>
       </c>
       <c r="AH245">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AI245" t="s">
         <v>50</v>
@@ -49468,7 +49468,7 @@
         <v>50</v>
       </c>
       <c r="AN245">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AP245">
         <v>0</v>
@@ -49477,13 +49477,13 @@
         <v>50</v>
       </c>
       <c r="AR245">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AS245" t="s">
         <v>50</v>
       </c>
       <c r="AT245">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AU245" t="s">
         <v>50</v>
@@ -50784,7 +50784,7 @@
         <v>46</v>
       </c>
       <c r="AV252">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AW252" t="s">
         <v>46</v>
@@ -51339,7 +51339,7 @@
         <v>46</v>
       </c>
       <c r="AV255">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AW255" t="s">
         <v>46</v>
@@ -51384,7 +51384,7 @@
         <v>46</v>
       </c>
       <c r="BL255">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BM255" t="s">
         <v>46</v>
@@ -51479,7 +51479,7 @@
         <v>46</v>
       </c>
       <c r="AF256">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AG256" t="s">
         <v>35</v>
@@ -51503,7 +51503,7 @@
         <v>46</v>
       </c>
       <c r="AN256">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AP256">
         <v>12</v>
@@ -52007,28 +52007,28 @@
         <v>46</v>
       </c>
       <c r="V259">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="W259" t="s">
         <v>46</v>
       </c>
       <c r="X259">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="Y259" t="s">
         <v>46</v>
       </c>
       <c r="Z259">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AB259">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AC259" t="s">
         <v>45</v>
       </c>
       <c r="AD259">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AE259" t="s">
         <v>35</v>
@@ -52091,46 +52091,46 @@
         <v>46</v>
       </c>
       <c r="AZ259">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BA259" t="s">
         <v>46</v>
       </c>
       <c r="BB259">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="BD259">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="BE259" t="s">
         <v>45</v>
       </c>
       <c r="BF259">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="BG259" t="s">
         <v>45</v>
       </c>
       <c r="BH259">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="BI259" t="s">
         <v>45</v>
       </c>
       <c r="BJ259">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="BK259" t="s">
         <v>45</v>
       </c>
       <c r="BL259">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="BM259" t="s">
         <v>45</v>
       </c>
       <c r="BN259">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="260" spans="1:66">
@@ -52741,7 +52741,7 @@
         <v>50</v>
       </c>
       <c r="T263">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="U263" t="s">
         <v>50</v>
@@ -53947,7 +53947,7 @@
         <v>46</v>
       </c>
       <c r="BB269">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BD269">
         <v>0</v>
@@ -54281,7 +54281,7 @@
         <v>4</v>
       </c>
       <c r="AP271">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="AQ271" t="s">
         <v>45</v>
@@ -56059,7 +56059,7 @@
         <v>50</v>
       </c>
       <c r="P281">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="Q281" t="s">
         <v>50</v>
@@ -56098,19 +56098,19 @@
         <v>50</v>
       </c>
       <c r="AD281">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AE281" t="s">
         <v>50</v>
       </c>
       <c r="AF281">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AG281" t="s">
         <v>50</v>
       </c>
       <c r="AH281">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AI281" t="s">
         <v>50</v>
@@ -56170,13 +56170,13 @@
         <v>5</v>
       </c>
       <c r="BD281">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="BE281" t="s">
         <v>50</v>
       </c>
       <c r="BF281">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BG281" t="s">
         <v>50</v>
@@ -56188,7 +56188,7 @@
         <v>50</v>
       </c>
       <c r="BJ281">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="BK281" t="s">
         <v>50</v>
@@ -56877,7 +56877,7 @@
         <v>46</v>
       </c>
       <c r="AR285">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AS285" t="s">
         <v>46</v>
@@ -57080,7 +57080,7 @@
         <v>46</v>
       </c>
       <c r="AX286">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AY286" t="s">
         <v>46</v>
@@ -58706,7 +58706,7 @@
         <v>50</v>
       </c>
       <c r="AJ295">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AK295" t="s">
         <v>50</v>
@@ -58772,7 +58772,7 @@
         <v>50</v>
       </c>
       <c r="BH295">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BI295" t="s">
         <v>50</v>
@@ -58784,7 +58784,7 @@
         <v>50</v>
       </c>
       <c r="BL295">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BM295" t="s">
         <v>50</v>
@@ -59183,7 +59183,7 @@
         <v>46</v>
       </c>
       <c r="H298">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I298" t="s">
         <v>36</v>
@@ -59434,64 +59434,64 @@
         <v>46</v>
       </c>
       <c r="AF299">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AG299" t="s">
         <v>46</v>
       </c>
       <c r="AH299">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AI299" t="s">
         <v>46</v>
       </c>
       <c r="AJ299">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AK299" t="s">
         <v>46</v>
       </c>
       <c r="AL299">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AM299" t="s">
         <v>46</v>
       </c>
       <c r="AN299">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AP299">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AQ299" t="s">
         <v>45</v>
       </c>
       <c r="AR299">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AS299" t="s">
         <v>45</v>
       </c>
       <c r="AT299">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AU299" t="s">
         <v>45</v>
       </c>
       <c r="AV299">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AW299" t="s">
         <v>45</v>
       </c>
       <c r="AX299">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AY299" t="s">
         <v>45</v>
       </c>
       <c r="AZ299">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BA299" t="s">
         <v>82</v>
@@ -59524,13 +59524,13 @@
         <v>46</v>
       </c>
       <c r="BL299">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BM299" t="s">
         <v>46</v>
       </c>
       <c r="BN299">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="300" spans="1:66">
@@ -59879,7 +59879,7 @@
         <v>46</v>
       </c>
       <c r="BF301">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BG301" t="s">
         <v>46</v>
@@ -62066,7 +62066,7 @@
         <v>50</v>
       </c>
       <c r="AT313">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AU313" t="s">
         <v>50</v>
@@ -63910,7 +63910,7 @@
         <v>46</v>
       </c>
       <c r="AR323">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="AS323" t="s">
         <v>46</v>
@@ -63940,7 +63940,7 @@
         <v>46</v>
       </c>
       <c r="BB323">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BD323">
         <v>0</v>
@@ -64125,7 +64125,7 @@
         <v>46</v>
       </c>
       <c r="BB324">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="BD324">
         <v>12</v>
@@ -64134,7 +64134,7 @@
         <v>46</v>
       </c>
       <c r="BF324">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="BG324" t="s">
         <v>46</v>
@@ -64304,7 +64304,7 @@
         <v>50</v>
       </c>
       <c r="AZ325">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BA325" t="s">
         <v>50</v>
@@ -64781,7 +64781,7 @@
         <v>50</v>
       </c>
       <c r="X328">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="Y328" t="s">
         <v>78</v>
@@ -64808,7 +64808,7 @@
         <v>50</v>
       </c>
       <c r="AH328">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AI328" t="s">
         <v>50</v>
@@ -64820,13 +64820,13 @@
         <v>50</v>
       </c>
       <c r="AL328">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AM328" t="s">
         <v>50</v>
       </c>
       <c r="AN328">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AP328">
         <v>0</v>
@@ -64880,13 +64880,13 @@
         <v>50</v>
       </c>
       <c r="BH328">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BI328" t="s">
         <v>46</v>
       </c>
       <c r="BJ328">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="BK328" t="s">
         <v>46</v>
@@ -65050,7 +65050,7 @@
         <v>46</v>
       </c>
       <c r="BB329">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="BD329">
         <v>0</v>
@@ -65387,7 +65387,7 @@
         <v>55</v>
       </c>
       <c r="AP331">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="AQ331" t="s">
         <v>50</v>
@@ -65933,7 +65933,7 @@
         <v>46</v>
       </c>
       <c r="AL334">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="AM334" t="s">
         <v>46</v>
@@ -68809,7 +68809,7 @@
         <v>46</v>
       </c>
       <c r="H350">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I350" t="s">
         <v>36</v>
@@ -68869,7 +68869,7 @@
         <v>46</v>
       </c>
       <c r="AD350">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AE350" t="s">
         <v>46</v>
@@ -69015,7 +69015,7 @@
         <v>45</v>
       </c>
       <c r="P351">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="Q351" t="s">
         <v>46</v>
@@ -69072,19 +69072,19 @@
         <v>46</v>
       </c>
       <c r="AJ351">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AK351" t="s">
         <v>46</v>
       </c>
       <c r="AL351">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AM351" t="s">
         <v>46</v>
       </c>
       <c r="AN351">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AP351">
         <v>0</v>
@@ -70104,7 +70104,7 @@
         <v>46</v>
       </c>
       <c r="H357">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I357" t="s">
         <v>36</v>
@@ -70209,7 +70209,7 @@
         <v>46</v>
       </c>
       <c r="AT357">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="AU357" t="s">
         <v>46</v>
@@ -70233,7 +70233,7 @@
         <v>46</v>
       </c>
       <c r="BB357">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="BD357">
         <v>12</v>
@@ -70937,7 +70937,7 @@
         <v>4</v>
       </c>
       <c r="AP361">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="AQ361" t="s">
         <v>35</v>
@@ -71125,7 +71125,7 @@
         <v>55</v>
       </c>
       <c r="AP362">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="AQ362" t="s">
         <v>50</v>
@@ -71817,7 +71817,7 @@
         <v>46</v>
       </c>
       <c r="X366">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="Y366" t="s">
         <v>35</v>
@@ -72650,7 +72650,7 @@
         <v>46</v>
       </c>
       <c r="BF370">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="BG370" t="s">
         <v>46</v>
@@ -72730,7 +72730,7 @@
         <v>46</v>
       </c>
       <c r="T371">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="U371" t="s">
         <v>46</v>
@@ -72781,7 +72781,7 @@
         <v>46</v>
       </c>
       <c r="AL371">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AM371" t="s">
         <v>35</v>
@@ -72987,7 +72987,7 @@
         <v>46</v>
       </c>
       <c r="AT372">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AU372" t="s">
         <v>46</v>
@@ -73133,7 +73133,7 @@
         <v>45</v>
       </c>
       <c r="AF373">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AG373" t="s">
         <v>45</v>
@@ -73172,7 +73172,7 @@
         <v>45</v>
       </c>
       <c r="AT373">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AU373" t="s">
         <v>45</v>
@@ -74383,25 +74383,25 @@
         <v>45</v>
       </c>
       <c r="P380">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="Q380" t="s">
         <v>45</v>
       </c>
       <c r="R380">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S380" t="s">
         <v>45</v>
       </c>
       <c r="T380">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="U380" t="s">
         <v>45</v>
       </c>
       <c r="V380">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="W380" t="s">
         <v>45</v>
@@ -74413,7 +74413,7 @@
         <v>45</v>
       </c>
       <c r="Z380">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AB380">
         <v>12</v>
@@ -74974,13 +74974,13 @@
         <v>55</v>
       </c>
       <c r="AB383">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AC383" t="s">
         <v>50</v>
       </c>
       <c r="AD383">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AE383" t="s">
         <v>50</v>
@@ -74998,7 +74998,7 @@
         <v>50</v>
       </c>
       <c r="AJ383">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AK383" t="s">
         <v>50</v>
@@ -75022,7 +75022,7 @@
         <v>50</v>
       </c>
       <c r="AR383">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="AS383" t="s">
         <v>50</v>
@@ -75034,7 +75034,7 @@
         <v>50</v>
       </c>
       <c r="AV383">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AW383" t="s">
         <v>50</v>
@@ -75052,7 +75052,7 @@
         <v>50</v>
       </c>
       <c r="BB383">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="BD383">
         <v>0</v>
@@ -75067,7 +75067,7 @@
         <v>50</v>
       </c>
       <c r="BH383">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="BI383" t="s">
         <v>50</v>
@@ -75848,7 +75848,7 @@
         <v>46</v>
       </c>
       <c r="H388">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I388" t="s">
         <v>36</v>
@@ -78152,7 +78152,7 @@
         <v>46</v>
       </c>
       <c r="AL400">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AM400" t="s">
         <v>46</v>
@@ -78492,7 +78492,7 @@
         <v>3</v>
       </c>
       <c r="AB402">
-        <v>12</v>
+        <v>11.5</v>
       </c>
       <c r="AC402" t="s">
         <v>45</v>
@@ -78549,7 +78549,7 @@
         <v>46</v>
       </c>
       <c r="AV402">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AW402" t="s">
         <v>46</v>
@@ -79289,7 +79289,7 @@
         <v>46</v>
       </c>
       <c r="AV406">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AW406" t="s">
         <v>46</v>
@@ -81234,7 +81234,7 @@
         <v>50</v>
       </c>
       <c r="P417">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="Q417" t="s">
         <v>46</v>
@@ -82383,7 +82383,7 @@
         <v>46</v>
       </c>
       <c r="AD423">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AE423" t="s">
         <v>46</v>
@@ -82753,7 +82753,7 @@
         <v>45</v>
       </c>
       <c r="AD425">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AE425" t="s">
         <v>45</v>
@@ -83472,7 +83472,7 @@
         <v>46</v>
       </c>
       <c r="V429">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="W429" t="s">
         <v>46</v>
@@ -83762,7 +83762,7 @@
         <v>45</v>
       </c>
       <c r="BH430">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BI430" t="s">
         <v>45</v>
@@ -83926,7 +83926,7 @@
         <v>45</v>
       </c>
       <c r="AZ431">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="BA431" t="s">
         <v>45</v>
@@ -84233,7 +84233,7 @@
         <v>50</v>
       </c>
       <c r="AD433">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AE433" t="s">
         <v>50</v>
@@ -84251,7 +84251,7 @@
         <v>50</v>
       </c>
       <c r="AJ433">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AK433" t="s">
         <v>50</v>
@@ -86068,7 +86068,7 @@
         <v>45</v>
       </c>
       <c r="X443">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="Y443" t="s">
         <v>45</v>
@@ -86089,7 +86089,7 @@
         <v>46</v>
       </c>
       <c r="AF443">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AG443" t="s">
         <v>46</v>
@@ -86444,7 +86444,7 @@
         <v>46</v>
       </c>
       <c r="Z445">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AB445">
         <v>0</v>
@@ -87748,13 +87748,13 @@
         <v>46</v>
       </c>
       <c r="AD452">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AE452" t="s">
         <v>46</v>
       </c>
       <c r="AF452">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AG452" t="s">
         <v>46</v>
@@ -87766,13 +87766,13 @@
         <v>46</v>
       </c>
       <c r="AJ452">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AK452" t="s">
         <v>46</v>
       </c>
       <c r="AL452">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AM452" t="s">
         <v>46</v>
@@ -87784,7 +87784,7 @@
         <v>55</v>
       </c>
       <c r="AP452">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="AQ452" t="s">
         <v>46</v>
@@ -87841,19 +87841,19 @@
         <v>46</v>
       </c>
       <c r="BJ452">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BK452" t="s">
         <v>46</v>
       </c>
       <c r="BL452">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="BM452" t="s">
         <v>46</v>
       </c>
       <c r="BN452">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="453" spans="1:66">
@@ -88112,7 +88112,7 @@
         <v>45</v>
       </c>
       <c r="Z454">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AB454">
         <v>12</v>
@@ -88151,7 +88151,7 @@
         <v>46</v>
       </c>
       <c r="AN454">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AP454">
         <v>0</v>
@@ -89377,7 +89377,7 @@
         <v>50</v>
       </c>
       <c r="P461">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="Q461" t="s">
         <v>50</v>
@@ -89401,7 +89401,7 @@
         <v>50</v>
       </c>
       <c r="X461">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="Y461" t="s">
         <v>50</v>
@@ -89434,7 +89434,7 @@
         <v>50</v>
       </c>
       <c r="AJ461">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AK461" t="s">
         <v>50</v>
@@ -89494,7 +89494,7 @@
         <v>50</v>
       </c>
       <c r="BF461">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BG461" t="s">
         <v>50</v>
@@ -91738,7 +91738,7 @@
         <v>50</v>
       </c>
       <c r="BN473">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="474" spans="1:66">
@@ -92624,7 +92624,7 @@
         <v>50</v>
       </c>
       <c r="AZ478">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BA478" t="s">
         <v>50</v>
@@ -92645,7 +92645,7 @@
         <v>50</v>
       </c>
       <c r="BH478">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BI478" t="s">
         <v>50</v>
@@ -93056,7 +93056,7 @@
         <v>46</v>
       </c>
       <c r="H481">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="I481" t="s">
         <v>36</v>
@@ -94647,7 +94647,7 @@
         <v>46</v>
       </c>
       <c r="AV489">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AW489" t="s">
         <v>46</v>
@@ -95130,7 +95130,7 @@
         <v>46</v>
       </c>
       <c r="V492">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="W492" t="s">
         <v>46</v>
@@ -95330,7 +95330,7 @@
         <v>4</v>
       </c>
       <c r="AB493">
-        <v>12</v>
+        <v>11.5</v>
       </c>
       <c r="AC493" t="s">
         <v>45</v>
@@ -95539,7 +95539,7 @@
         <v>46</v>
       </c>
       <c r="AJ494">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AK494" t="s">
         <v>46</v>
@@ -95551,7 +95551,7 @@
         <v>46</v>
       </c>
       <c r="AN494">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AP494">
         <v>0</v>
@@ -95560,7 +95560,7 @@
         <v>46</v>
       </c>
       <c r="AR494">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AS494" t="s">
         <v>35</v>
@@ -96216,7 +96216,7 @@
         <v>0</v>
       </c>
       <c r="N498">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="O498" t="s">
         <v>45</v>
@@ -96267,7 +96267,7 @@
         <v>46</v>
       </c>
       <c r="AF498">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AG498" t="s">
         <v>46</v>
@@ -96279,52 +96279,52 @@
         <v>46</v>
       </c>
       <c r="AJ498">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AK498" t="s">
         <v>46</v>
       </c>
       <c r="AL498">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AM498" t="s">
         <v>46</v>
       </c>
       <c r="AN498">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AP498">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AQ498" t="s">
         <v>45</v>
       </c>
       <c r="AR498">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AS498" t="s">
         <v>45</v>
       </c>
       <c r="AT498">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AU498" t="s">
         <v>45</v>
       </c>
       <c r="AV498">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AW498" t="s">
         <v>45</v>
       </c>
       <c r="AX498">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AY498" t="s">
         <v>45</v>
       </c>
       <c r="AZ498">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BA498" t="s">
         <v>82</v>
@@ -96339,13 +96339,13 @@
         <v>46</v>
       </c>
       <c r="BF498">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BG498" t="s">
         <v>46</v>
       </c>
       <c r="BH498">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BI498" t="s">
         <v>46</v>
@@ -96357,13 +96357,13 @@
         <v>46</v>
       </c>
       <c r="BL498">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BM498" t="s">
         <v>46</v>
       </c>
       <c r="BN498">
-        <v>4</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="499" spans="1:66">
@@ -96941,7 +96941,7 @@
         <v>46</v>
       </c>
       <c r="H502">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I502" t="s">
         <v>36</v>
@@ -97404,7 +97404,7 @@
         <v>4</v>
       </c>
       <c r="AP504">
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="AQ504" t="s">
         <v>45</v>
@@ -98451,7 +98451,7 @@
         <v>46</v>
       </c>
       <c r="Z510">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AB510">
         <v>0</v>
@@ -98490,7 +98490,7 @@
         <v>46</v>
       </c>
       <c r="AN510">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AP510">
         <v>0</v>
@@ -98928,7 +98928,7 @@
         <v>0</v>
       </c>
       <c r="AB513">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="AC513" t="s">
         <v>50</v>
@@ -99223,13 +99223,13 @@
         <v>46</v>
       </c>
       <c r="V515">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="W515" t="s">
         <v>46</v>
       </c>
       <c r="X515">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Y515" t="s">
         <v>46</v>
@@ -100576,7 +100576,7 @@
         <v>46</v>
       </c>
       <c r="BL530">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="BM530" t="s">
         <v>46</v>
@@ -100611,13 +100611,13 @@
         <v>46</v>
       </c>
       <c r="BL531">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="BM531" t="s">
         <v>46</v>
       </c>
       <c r="BN531">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="532" spans="1:66">
@@ -101083,7 +101083,7 @@
         <v>46</v>
       </c>
       <c r="R536">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="S536" t="s">
         <v>46</v>
@@ -102390,19 +102390,19 @@
         <v>46</v>
       </c>
       <c r="V543">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="W543" t="s">
         <v>46</v>
       </c>
       <c r="X543">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="Y543" t="s">
         <v>46</v>
       </c>
       <c r="Z543">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AB543">
         <v>12</v>
@@ -102411,7 +102411,7 @@
         <v>45</v>
       </c>
       <c r="AD543">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AE543" t="s">
         <v>45</v>
@@ -104694,13 +104694,13 @@
         <v>46</v>
       </c>
       <c r="AZ555">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="BA555" t="s">
         <v>46</v>
       </c>
       <c r="BB555">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="BD555">
         <v>12</v>
@@ -104721,19 +104721,19 @@
         <v>46</v>
       </c>
       <c r="BJ555">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BK555" t="s">
         <v>46</v>
       </c>
       <c r="BL555">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BM555" t="s">
         <v>46</v>
       </c>
       <c r="BN555">
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="556" spans="1:66">
@@ -104995,7 +104995,7 @@
         <v>0</v>
       </c>
       <c r="AB557">
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="AC557" t="s">
         <v>50</v>
@@ -105040,7 +105040,7 @@
         <v>50</v>
       </c>
       <c r="AR557">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="AS557" t="s">
         <v>50</v>
@@ -105058,7 +105058,7 @@
         <v>50</v>
       </c>
       <c r="AX557">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AY557" t="s">
         <v>78</v>
@@ -105147,25 +105147,25 @@
         <v>50</v>
       </c>
       <c r="P558">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="Q558" t="s">
         <v>50</v>
       </c>
       <c r="R558">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S558" t="s">
         <v>50</v>
       </c>
       <c r="T558">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="U558" t="s">
         <v>50</v>
       </c>
       <c r="V558">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="W558" t="s">
         <v>50</v>
@@ -105177,7 +105177,7 @@
         <v>50</v>
       </c>
       <c r="Z558">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AB558">
         <v>0</v>
@@ -105186,7 +105186,7 @@
         <v>50</v>
       </c>
       <c r="AD558">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AE558" t="s">
         <v>50</v>
@@ -105198,19 +105198,19 @@
         <v>50</v>
       </c>
       <c r="AH558">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AI558" t="s">
         <v>50</v>
       </c>
       <c r="AJ558">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AK558" t="s">
         <v>50</v>
       </c>
       <c r="AL558">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AM558" t="s">
         <v>50</v>
@@ -105231,25 +105231,25 @@
         <v>50</v>
       </c>
       <c r="AT558">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AU558" t="s">
         <v>50</v>
       </c>
       <c r="AV558">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AW558" t="s">
         <v>50</v>
       </c>
       <c r="AX558">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AY558" t="s">
         <v>50</v>
       </c>
       <c r="AZ558">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BA558" t="s">
         <v>50</v>
@@ -105264,19 +105264,19 @@
         <v>50</v>
       </c>
       <c r="BF558">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BG558" t="s">
         <v>50</v>
       </c>
       <c r="BH558">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BI558" t="s">
         <v>50</v>
       </c>
       <c r="BJ558">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="BK558" t="s">
         <v>50</v>
@@ -105288,7 +105288,7 @@
         <v>50</v>
       </c>
       <c r="BN558">
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="559" spans="1:66">
@@ -105920,7 +105920,7 @@
         <v>0</v>
       </c>
       <c r="AB562">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="AC562" t="s">
         <v>50</v>
@@ -105995,7 +105995,7 @@
         <v>46</v>
       </c>
       <c r="BB562">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="BD562">
         <v>0</v>
@@ -106511,7 +106511,7 @@
         <v>46</v>
       </c>
       <c r="AN565">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AP565">
         <v>0</v>
@@ -106532,19 +106532,19 @@
         <v>46</v>
       </c>
       <c r="AV565">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AW565" t="s">
         <v>46</v>
       </c>
       <c r="AX565">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AY565" t="s">
         <v>46</v>
       </c>
       <c r="AZ565">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BA565" t="s">
         <v>35</v>
@@ -106830,7 +106830,7 @@
         <v>46</v>
       </c>
       <c r="V567">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="W567" t="s">
         <v>46</v>
@@ -107367,31 +107367,31 @@
         <v>46</v>
       </c>
       <c r="P570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="Q570" t="s">
         <v>46</v>
       </c>
       <c r="R570">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="S570" t="s">
         <v>46</v>
       </c>
       <c r="T570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="U570" t="s">
         <v>46</v>
       </c>
       <c r="V570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="W570" t="s">
         <v>46</v>
       </c>
       <c r="X570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="Y570" t="s">
         <v>46</v>
@@ -107400,19 +107400,19 @@
         <v>3</v>
       </c>
       <c r="AB570">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AC570" t="s">
         <v>45</v>
       </c>
       <c r="AD570">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AE570" t="s">
         <v>45</v>
       </c>
       <c r="AF570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AG570" t="s">
         <v>45</v>
@@ -107424,13 +107424,13 @@
         <v>45</v>
       </c>
       <c r="AJ570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AK570" t="s">
         <v>45</v>
       </c>
       <c r="AL570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AM570" t="s">
         <v>45</v>
@@ -107439,76 +107439,76 @@
         <v>4</v>
       </c>
       <c r="AP570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AQ570" t="s">
         <v>46</v>
       </c>
       <c r="AR570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AS570" t="s">
         <v>46</v>
       </c>
       <c r="AT570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AU570" t="s">
         <v>46</v>
       </c>
       <c r="AV570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AW570" t="s">
         <v>46</v>
       </c>
       <c r="AX570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AY570" t="s">
         <v>46</v>
       </c>
       <c r="AZ570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BA570" t="s">
         <v>46</v>
       </c>
       <c r="BB570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BD570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BE570" t="s">
         <v>45</v>
       </c>
       <c r="BF570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BG570" t="s">
         <v>45</v>
       </c>
       <c r="BH570">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="BI570" t="s">
         <v>45</v>
       </c>
       <c r="BJ570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BK570" t="s">
         <v>45</v>
       </c>
       <c r="BL570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BM570" t="s">
         <v>45</v>
       </c>
       <c r="BN570">
-        <v>4</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="571" spans="1:66">
@@ -108086,7 +108086,7 @@
         <v>46</v>
       </c>
       <c r="H574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="I574" t="s">
         <v>36</v>
@@ -108107,25 +108107,25 @@
         <v>45</v>
       </c>
       <c r="P574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="Q574" t="s">
         <v>45</v>
       </c>
       <c r="R574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S574" t="s">
         <v>45</v>
       </c>
       <c r="T574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="U574" t="s">
         <v>45</v>
       </c>
       <c r="V574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="W574" t="s">
         <v>45</v>
@@ -108152,85 +108152,85 @@
         <v>46</v>
       </c>
       <c r="AF574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AG574" t="s">
         <v>46</v>
       </c>
       <c r="AH574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AI574" t="s">
         <v>46</v>
       </c>
       <c r="AJ574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AK574" t="s">
         <v>46</v>
       </c>
       <c r="AL574">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AM574" t="s">
         <v>46</v>
       </c>
       <c r="AN574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AP574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AQ574" t="s">
         <v>45</v>
       </c>
       <c r="AR574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AS574" t="s">
         <v>45</v>
       </c>
       <c r="AT574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AU574" t="s">
         <v>45</v>
       </c>
       <c r="AV574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AW574" t="s">
         <v>45</v>
       </c>
       <c r="AX574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AY574" t="s">
         <v>45</v>
       </c>
       <c r="AZ574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BA574" t="s">
         <v>45</v>
       </c>
       <c r="BB574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BD574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BE574" t="s">
         <v>46</v>
       </c>
       <c r="BF574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BG574" t="s">
         <v>46</v>
       </c>
       <c r="BH574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BI574" t="s">
         <v>46</v>
@@ -108242,13 +108242,13 @@
         <v>46</v>
       </c>
       <c r="BL574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BM574" t="s">
         <v>46</v>
       </c>
       <c r="BN574">
-        <v>4</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="575" spans="1:66">
@@ -109038,13 +109038,13 @@
         <v>46</v>
       </c>
       <c r="R579">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="S579" t="s">
         <v>46</v>
       </c>
       <c r="T579">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="U579" t="s">
         <v>46</v>
@@ -109951,37 +109951,37 @@
         <v>0</v>
       </c>
       <c r="N584">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="O584" t="s">
         <v>45</v>
       </c>
       <c r="P584">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="Q584" t="s">
         <v>45</v>
       </c>
       <c r="R584">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S584" t="s">
         <v>45</v>
       </c>
       <c r="T584">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="U584" t="s">
         <v>45</v>
       </c>
       <c r="V584">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="W584" t="s">
         <v>45</v>
       </c>
       <c r="X584">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="Y584" t="s">
         <v>45</v>
@@ -109990,7 +109990,7 @@
         <v>4</v>
       </c>
       <c r="AB584">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AC584" t="s">
         <v>46</v>
@@ -110035,7 +110035,7 @@
         <v>45</v>
       </c>
       <c r="AR584">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AS584" t="s">
         <v>82</v>
@@ -110053,7 +110053,7 @@
         <v>45</v>
       </c>
       <c r="AX584">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AY584" t="s">
         <v>45</v>
@@ -110277,7 +110277,7 @@
         <v>46</v>
       </c>
       <c r="BL585">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BM585" t="s">
         <v>46</v>
@@ -111073,7 +111073,7 @@
         <v>50</v>
       </c>
       <c r="R590">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S590" t="s">
         <v>50</v>
@@ -111786,7 +111786,7 @@
         <v>46</v>
       </c>
       <c r="H594">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="I594" t="s">
         <v>36</v>
@@ -111807,7 +111807,7 @@
         <v>46</v>
       </c>
       <c r="P594">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="Q594" t="s">
         <v>46</v>
@@ -111819,7 +111819,7 @@
         <v>46</v>
       </c>
       <c r="T594">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="U594" t="s">
         <v>46</v>
@@ -111876,7 +111876,7 @@
         <v>46</v>
       </c>
       <c r="AN594">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AP594">
         <v>11</v>
@@ -111915,7 +111915,7 @@
         <v>46</v>
       </c>
       <c r="BB594">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BD594">
         <v>11</v>
@@ -112210,7 +112210,7 @@
         <v>0</v>
       </c>
       <c r="AB596">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="AC596" t="s">
         <v>50</v>
@@ -112228,7 +112228,7 @@
         <v>50</v>
       </c>
       <c r="AH596">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AI596" t="s">
         <v>50</v>
@@ -112255,13 +112255,13 @@
         <v>50</v>
       </c>
       <c r="AR596">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="AS596" t="s">
         <v>50</v>
       </c>
       <c r="AT596">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AU596" t="s">
         <v>50</v>
@@ -112288,7 +112288,7 @@
         <v>0</v>
       </c>
       <c r="BD596">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="BE596" t="s">
         <v>50</v>
@@ -112870,7 +112870,7 @@
         <v>46</v>
       </c>
       <c r="BL599">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BM599" t="s">
         <v>46</v>
@@ -113454,7 +113454,7 @@
         <v>46</v>
       </c>
       <c r="H603">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I603" t="s">
         <v>36</v>
@@ -113639,7 +113639,7 @@
         <v>45</v>
       </c>
       <c r="H604">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="I604" t="s">
         <v>36</v>
@@ -114278,7 +114278,7 @@
         <v>46</v>
       </c>
       <c r="AL607">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AM607" t="s">
         <v>46</v>
@@ -114394,7 +114394,7 @@
         <v>0</v>
       </c>
       <c r="N608">
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="O608" t="s">
         <v>35</v>
@@ -114463,7 +114463,7 @@
         <v>46</v>
       </c>
       <c r="AL608">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AM608" t="s">
         <v>46</v>
@@ -115889,7 +115889,7 @@
         <v>46</v>
       </c>
       <c r="R616">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="S616" t="s">
         <v>46</v>
@@ -115901,7 +115901,7 @@
         <v>46</v>
       </c>
       <c r="V616">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="W616" t="s">
         <v>46</v>
@@ -117647,13 +117647,13 @@
         <v>46</v>
       </c>
       <c r="BH634">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BI634" t="s">
         <v>46</v>
       </c>
       <c r="BJ634">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BK634" t="s">
         <v>46</v>
@@ -117665,7 +117665,7 @@
         <v>46</v>
       </c>
       <c r="BN634">
-        <v>4</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="635" spans="1:66">

</xml_diff>